<commit_message>
power rankings austria r
</commit_message>
<xml_diff>
--- a/The Alternative F1 Season 4 Power Rankings (Responses).xlsx
+++ b/The Alternative F1 Season 4 Power Rankings (Responses).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
   <si>
     <t>Timestamp</t>
   </si>
@@ -98,10 +98,10 @@
     <t>Mexico</t>
   </si>
   <si>
-    <t>Balu</t>
+    <t>Baku</t>
   </si>
   <si>
-    <t>Baku</t>
+    <t>Austria R</t>
   </si>
   <si>
     <t>Race</t>
@@ -258,7 +258,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I25" displayName="Form_Responses" name="Form_Responses" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I28" displayName="Form_Responses" name="Form_Responses" id="1">
   <tableColumns count="9">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -1217,6 +1217,93 @@
         <v>1.0</v>
       </c>
     </row>
+    <row r="26" ht="22.5" customHeight="1">
+      <c r="A26" s="4">
+        <v>45973.903830138894</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D26" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="H26" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="I26" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="27" ht="22.5" customHeight="1">
+      <c r="A27" s="4">
+        <v>45973.90955939815</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="H27" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="I27" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="28" ht="22.5" customHeight="1">
+      <c r="A28" s="4">
+        <v>45973.94470622685</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="H28" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="I28" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -1428,31 +1515,31 @@
         <v>26</v>
       </c>
       <c r="B7" s="7">
-        <f>AVERAGE('Form Responses 1'!C19:C28)</f>
-        <v>3.857142857</v>
+        <f>AVERAGE('Form Responses 1'!C19:C31)</f>
+        <v>3.6</v>
       </c>
       <c r="C7" s="7">
-        <f>AVERAGE('Form Responses 1'!D19:D28)</f>
-        <v>3.571428571</v>
+        <f>AVERAGE('Form Responses 1'!D19:D31)</f>
+        <v>3.6</v>
       </c>
       <c r="D7" s="7">
-        <f>AVERAGE('Form Responses 1'!E19:E28)</f>
-        <v>3.142857143</v>
+        <f>AVERAGE('Form Responses 1'!E19:E31)</f>
+        <v>2.9</v>
       </c>
       <c r="E7" s="7">
-        <f>AVERAGE('Form Responses 1'!F19:F28)</f>
+        <f>AVERAGE('Form Responses 1'!F19:F31)</f>
         <v>6</v>
       </c>
       <c r="F7" s="7">
-        <f>AVERAGE('Form Responses 1'!G19:G28)</f>
-        <v>5.857142857</v>
+        <f>AVERAGE('Form Responses 1'!G19:G31)</f>
+        <v>5.8</v>
       </c>
       <c r="G7" s="7">
-        <f>AVERAGE('Form Responses 1'!H19:H28)</f>
-        <v>4.571428571</v>
+        <f>AVERAGE('Form Responses 1'!H19:H31)</f>
+        <v>5.1</v>
       </c>
       <c r="H7" s="7">
-        <f>AVERAGE('Form Responses 1'!I19:I28)</f>
+        <f>AVERAGE('Form Responses 1'!I19:I31)</f>
         <v>1</v>
       </c>
     </row>
@@ -1486,6 +1573,39 @@
       </c>
       <c r="H8" s="7">
         <f>AVERAGE('Form Responses 1'!I22:I25)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="7">
+        <f>AVERAGE('Form Responses 1'!C26:C28)</f>
+        <v>3</v>
+      </c>
+      <c r="C9" s="7">
+        <f>AVERAGE('Form Responses 1'!D26:D28)</f>
+        <v>3.666666667</v>
+      </c>
+      <c r="D9" s="7">
+        <f>AVERAGE('Form Responses 1'!E26:E28)</f>
+        <v>2.333333333</v>
+      </c>
+      <c r="E9" s="7">
+        <f>AVERAGE('Form Responses 1'!F26:F28)</f>
+        <v>6</v>
+      </c>
+      <c r="F9" s="7">
+        <f>AVERAGE('Form Responses 1'!G26:G28)</f>
+        <v>5.666666667</v>
+      </c>
+      <c r="G9" s="7">
+        <f>AVERAGE('Form Responses 1'!H26:H28)</f>
+        <v>6.333333333</v>
+      </c>
+      <c r="H9" s="7">
+        <f>AVERAGE('Form Responses 1'!I26:I28)</f>
         <v>1</v>
       </c>
     </row>
@@ -1698,15 +1818,15 @@
       </c>
       <c r="B7" s="7">
         <f>AVERAGE('Ranking Per Race'!B$2:B7)</f>
-        <v>2.406746032</v>
+        <v>2.363888889</v>
       </c>
       <c r="C7" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C7)</f>
-        <v>2.900793651</v>
+        <v>2.905555556</v>
       </c>
       <c r="D7" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D7)</f>
-        <v>3.037698413</v>
+        <v>2.997222222</v>
       </c>
       <c r="E7" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E7)</f>
@@ -1714,11 +1834,11 @@
       </c>
       <c r="F7" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F7)</f>
-        <v>5.392857143</v>
+        <v>5.383333333</v>
       </c>
       <c r="G7" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G7)</f>
-        <v>4.386904762</v>
+        <v>4.475</v>
       </c>
       <c r="H7" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H7)</f>
@@ -1727,19 +1847,19 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="7">
         <f>AVERAGE('Ranking Per Race'!B$2:B8)</f>
-        <v>2.455782313</v>
+        <v>2.419047619</v>
       </c>
       <c r="C8" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C8)</f>
-        <v>3.022108844</v>
+        <v>3.026190476</v>
       </c>
       <c r="D8" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D8)</f>
-        <v>3.175170068</v>
+        <v>3.14047619</v>
       </c>
       <c r="E8" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E8)</f>
@@ -1747,15 +1867,48 @@
       </c>
       <c r="F8" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F8)</f>
-        <v>5.551020408</v>
+        <v>5.542857143</v>
       </c>
       <c r="G8" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G8)</f>
-        <v>4.43877551</v>
+        <v>4.514285714</v>
       </c>
       <c r="H8" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H8)</f>
         <v>3.797619048</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="7">
+        <f>AVERAGE('Ranking Per Race'!B$2:B9)</f>
+        <v>2.491666667</v>
+      </c>
+      <c r="C9" s="7">
+        <f>AVERAGE('Ranking Per Race'!C$2:C9)</f>
+        <v>3.10625</v>
+      </c>
+      <c r="D9" s="7">
+        <f>AVERAGE('Ranking Per Race'!D$2:D9)</f>
+        <v>3.039583333</v>
+      </c>
+      <c r="E9" s="7">
+        <f>AVERAGE('Ranking Per Race'!E$2:E9)</f>
+        <v>5.614583333</v>
+      </c>
+      <c r="F9" s="7">
+        <f>AVERAGE('Ranking Per Race'!F$2:F9)</f>
+        <v>5.558333333</v>
+      </c>
+      <c r="G9" s="7">
+        <f>AVERAGE('Ranking Per Race'!G$2:G9)</f>
+        <v>4.741666667</v>
+      </c>
+      <c r="H9" s="7">
+        <f>AVERAGE('Ranking Per Race'!H$2:H9)</f>
+        <v>3.447916667</v>
       </c>
     </row>
   </sheetData>
@@ -1970,15 +2123,15 @@
       </c>
       <c r="B7" s="7">
         <f>AVERAGE('Average Ranking'!B$2:B7)</f>
-        <v>1.750429894</v>
+        <v>1.743287037</v>
       </c>
       <c r="C7" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C7)</f>
-        <v>2.548743386</v>
+        <v>2.549537037</v>
       </c>
       <c r="D7" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D7)</f>
-        <v>3.151421958</v>
+        <v>3.144675926</v>
       </c>
       <c r="E7" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E7)</f>
@@ -1986,11 +2139,11 @@
       </c>
       <c r="F7" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F7)</f>
-        <v>5.164087302</v>
+        <v>5.1625</v>
       </c>
       <c r="G7" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G7)</f>
-        <v>4.945734127</v>
+        <v>4.960416667</v>
       </c>
       <c r="H7" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H7)</f>
@@ -1999,19 +2152,19 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="7">
         <f>AVERAGE('Average Ranking'!B$2:B8)</f>
-        <v>1.851194525</v>
+        <v>1.839824263</v>
       </c>
       <c r="C8" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C8)</f>
-        <v>2.616367023</v>
+        <v>2.617630385</v>
       </c>
       <c r="D8" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D8)</f>
-        <v>3.154814545</v>
+        <v>3.144075964</v>
       </c>
       <c r="E8" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E8)</f>
@@ -2019,15 +2172,48 @@
       </c>
       <c r="F8" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F8)</f>
-        <v>5.21936346</v>
+        <v>5.216836735</v>
       </c>
       <c r="G8" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G8)</f>
-        <v>4.873311467</v>
+        <v>4.896683673</v>
       </c>
       <c r="H8" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H8)</f>
         <v>4.946286848</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="7">
+        <f>AVERAGE('Average Ranking'!B$2:B9)</f>
+        <v>1.921304563</v>
+      </c>
+      <c r="C9" s="7">
+        <f>AVERAGE('Average Ranking'!C$2:C9)</f>
+        <v>2.678707837</v>
+      </c>
+      <c r="D9" s="7">
+        <f>AVERAGE('Average Ranking'!D$2:D9)</f>
+        <v>3.131014385</v>
+      </c>
+      <c r="E9" s="7">
+        <f>AVERAGE('Average Ranking'!E$2:E9)</f>
+        <v>5.373152282</v>
+      </c>
+      <c r="F9" s="7">
+        <f>AVERAGE('Average Ranking'!F$2:F9)</f>
+        <v>5.25952381</v>
+      </c>
+      <c r="G9" s="7">
+        <f>AVERAGE('Average Ranking'!G$2:G9)</f>
+        <v>4.877306548</v>
+      </c>
+      <c r="H9" s="7">
+        <f>AVERAGE('Average Ranking'!H$2:H9)</f>
+        <v>4.758990575</v>
       </c>
     </row>
   </sheetData>
@@ -2309,32 +2495,28 @@
     <row r="9">
       <c r="A9" s="6" t="str">
         <f>'Pre-Final Ranking'!A9</f>
-        <v/>
-      </c>
-      <c r="B9" s="6" t="str">
-        <f>'Pre-Final Ranking'!B9</f>
-        <v/>
-      </c>
-      <c r="C9" s="6" t="str">
-        <f>'Pre-Final Ranking'!C9</f>
-        <v/>
-      </c>
-      <c r="D9" s="6" t="str">
-        <f>'Pre-Final Ranking'!D9</f>
-        <v/>
-      </c>
-      <c r="E9" s="6" t="str">
-        <f>'Pre-Final Ranking'!E9</f>
-        <v/>
-      </c>
-      <c r="F9" s="6" t="str">
-        <f>'Pre-Final Ranking'!F9</f>
-        <v/>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6" t="str">
-        <f>'Pre-Final Ranking'!H9</f>
-        <v/>
+        <v>Austria R</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="C9" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>3.0</v>
       </c>
       <c r="I9" s="6" t="str">
         <f>'Pre-Final Ranking'!I9</f>

</xml_diff>

<commit_message>
power rankings for brazil and austria
</commit_message>
<xml_diff>
--- a/The Alternative F1 Season 4 Power Rankings (Responses).xlsx
+++ b/The Alternative F1 Season 4 Power Rankings (Responses).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="34">
   <si>
     <t>Timestamp</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>Spa</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Austria</t>
   </si>
   <si>
     <t>Race</t>
@@ -261,7 +267,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I30" displayName="Form_Responses" name="Form_Responses" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I35" displayName="Form_Responses" name="Form_Responses" id="1">
   <tableColumns count="9">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -1365,6 +1371,151 @@
         <v>2.0</v>
       </c>
     </row>
+    <row r="31" ht="22.5" customHeight="1">
+      <c r="A31" s="4">
+        <v>45996.784788530094</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D31" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="F31" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="G31" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="H31" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="I31" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="32" ht="22.5" customHeight="1">
+      <c r="A32" s="4">
+        <v>45996.78592445602</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D32" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E32" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="G32" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="H32" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="I32" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="33" ht="22.5" customHeight="1">
+      <c r="A33" s="4">
+        <v>45999.4195668287</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D33" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="E33" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="F33" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="G33" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="H33" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="I33" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="34" ht="22.5" customHeight="1">
+      <c r="A34" s="4">
+        <v>46001.91722189815</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D34" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E34" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="F34" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="G34" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="H34" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="I34" s="5">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="35" ht="22.5" customHeight="1">
+      <c r="A35" s="4">
+        <v>46001.91853622685</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D35" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="E35" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="F35" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="G35" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="H35" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="I35" s="5">
+        <v>3.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -1576,32 +1727,32 @@
         <v>26</v>
       </c>
       <c r="B7" s="7">
-        <f>AVERAGE('Form Responses 1'!C19:C33)</f>
-        <v>3.5</v>
+        <f>AVERAGE('Form Responses 1'!C19:C38)</f>
+        <v>3.176470588</v>
       </c>
       <c r="C7" s="7">
-        <f>AVERAGE('Form Responses 1'!D19:D33)</f>
-        <v>3.666666667</v>
+        <f>AVERAGE('Form Responses 1'!D19:D38)</f>
+        <v>4.117647059</v>
       </c>
       <c r="D7" s="7">
-        <f>AVERAGE('Form Responses 1'!E19:E33)</f>
-        <v>2.583333333</v>
+        <f>AVERAGE('Form Responses 1'!E19:E38)</f>
+        <v>2.235294118</v>
       </c>
       <c r="E7" s="7">
-        <f>AVERAGE('Form Responses 1'!F19:F33)</f>
-        <v>5.916666667</v>
+        <f>AVERAGE('Form Responses 1'!F19:F38)</f>
+        <v>5.823529412</v>
       </c>
       <c r="F7" s="7">
-        <f>AVERAGE('Form Responses 1'!G19:G33)</f>
-        <v>6</v>
+        <f>AVERAGE('Form Responses 1'!G19:G38)</f>
+        <v>6.058823529</v>
       </c>
       <c r="G7" s="7">
-        <f>AVERAGE('Form Responses 1'!H19:H33)</f>
-        <v>5.166666667</v>
+        <f>AVERAGE('Form Responses 1'!H19:H38)</f>
+        <v>5</v>
       </c>
       <c r="H7" s="7">
-        <f>AVERAGE('Form Responses 1'!I19:I33)</f>
-        <v>1.166666667</v>
+        <f>AVERAGE('Form Responses 1'!I19:I38)</f>
+        <v>1.588235294</v>
       </c>
     </row>
     <row r="8">
@@ -1701,6 +1852,72 @@
       <c r="H10" s="7">
         <f>AVERAGE('Form Responses 1'!I29:I30)</f>
         <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="7">
+        <f>AVERAGE('Form Responses 1'!C31:C33)</f>
+        <v>2.666666667</v>
+      </c>
+      <c r="C11" s="7">
+        <f>AVERAGE('Form Responses 1'!D31:D33)</f>
+        <v>4.666666667</v>
+      </c>
+      <c r="D11" s="7">
+        <f>AVERAGE('Form Responses 1'!E31:E33)</f>
+        <v>1.666666667</v>
+      </c>
+      <c r="E11" s="7">
+        <f>AVERAGE('Form Responses 1'!F31:F33)</f>
+        <v>5.333333333</v>
+      </c>
+      <c r="F11" s="7">
+        <f>AVERAGE('Form Responses 1'!G31:G33)</f>
+        <v>6.666666667</v>
+      </c>
+      <c r="G11" s="7">
+        <f>AVERAGE('Form Responses 1'!H31:H33)</f>
+        <v>4.666666667</v>
+      </c>
+      <c r="H11" s="7">
+        <f>AVERAGE('Form Responses 1'!I31:I33)</f>
+        <v>2.333333333</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="7">
+        <f>AVERAGE('Form Responses 1'!C34:C35)</f>
+        <v>2</v>
+      </c>
+      <c r="C12" s="7">
+        <f>AVERAGE('Form Responses 1'!D34:D35)</f>
+        <v>6</v>
+      </c>
+      <c r="D12" s="7">
+        <f>AVERAGE('Form Responses 1'!E34:E35)</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="7">
+        <f>AVERAGE('Form Responses 1'!F34:F35)</f>
+        <v>6</v>
+      </c>
+      <c r="F12" s="7">
+        <f>AVERAGE('Form Responses 1'!G34:G35)</f>
+        <v>5.5</v>
+      </c>
+      <c r="G12" s="7">
+        <f>AVERAGE('Form Responses 1'!H34:H35)</f>
+        <v>4.5</v>
+      </c>
+      <c r="H12" s="7">
+        <f>AVERAGE('Form Responses 1'!I34:I35)</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1912,31 +2129,31 @@
       </c>
       <c r="B7" s="7">
         <f>AVERAGE('Ranking Per Race'!B$2:B7)</f>
-        <v>2.347222222</v>
+        <v>2.293300654</v>
       </c>
       <c r="C7" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C7)</f>
-        <v>2.916666667</v>
+        <v>2.991830065</v>
       </c>
       <c r="D7" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D7)</f>
-        <v>2.944444444</v>
+        <v>2.886437908</v>
       </c>
       <c r="E7" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E7)</f>
-        <v>5.597222222</v>
+        <v>5.581699346</v>
       </c>
       <c r="F7" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F7)</f>
-        <v>5.416666667</v>
+        <v>5.426470588</v>
       </c>
       <c r="G7" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G7)</f>
-        <v>4.486111111</v>
+        <v>4.458333333</v>
       </c>
       <c r="H7" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H7)</f>
-        <v>4.291666667</v>
+        <v>4.361928105</v>
       </c>
     </row>
     <row r="8">
@@ -1945,31 +2162,31 @@
       </c>
       <c r="B8" s="7">
         <f>AVERAGE('Ranking Per Race'!B$2:B8)</f>
-        <v>2.404761905</v>
+        <v>2.358543417</v>
       </c>
       <c r="C8" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C8)</f>
-        <v>3.035714286</v>
+        <v>3.100140056</v>
       </c>
       <c r="D8" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D8)</f>
-        <v>3.095238095</v>
+        <v>3.045518207</v>
       </c>
       <c r="E8" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E8)</f>
-        <v>5.547619048</v>
+        <v>5.534313725</v>
       </c>
       <c r="F8" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F8)</f>
-        <v>5.571428571</v>
+        <v>5.579831933</v>
       </c>
       <c r="G8" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G8)</f>
-        <v>4.523809524</v>
+        <v>4.5</v>
       </c>
       <c r="H8" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H8)</f>
-        <v>3.821428571</v>
+        <v>3.881652661</v>
       </c>
     </row>
     <row r="9">
@@ -1978,31 +2195,31 @@
       </c>
       <c r="B9" s="7">
         <f>AVERAGE('Ranking Per Race'!B$2:B9)</f>
-        <v>2.479166667</v>
+        <v>2.43872549</v>
       </c>
       <c r="C9" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C9)</f>
-        <v>3.114583333</v>
+        <v>3.170955882</v>
       </c>
       <c r="D9" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D9)</f>
-        <v>3</v>
+        <v>2.956495098</v>
       </c>
       <c r="E9" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E9)</f>
-        <v>5.604166667</v>
+        <v>5.59252451</v>
       </c>
       <c r="F9" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F9)</f>
-        <v>5.583333333</v>
+        <v>5.590686275</v>
       </c>
       <c r="G9" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G9)</f>
-        <v>4.75</v>
+        <v>4.729166667</v>
       </c>
       <c r="H9" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H9)</f>
-        <v>3.46875</v>
+        <v>3.521446078</v>
       </c>
     </row>
     <row r="10">
@@ -2011,31 +2228,97 @@
       </c>
       <c r="B10" s="7">
         <f>AVERAGE('Ranking Per Race'!B$2:B10)</f>
-        <v>2.537037037</v>
+        <v>2.501089325</v>
       </c>
       <c r="C10" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C10)</f>
-        <v>3.212962963</v>
+        <v>3.263071895</v>
       </c>
       <c r="D10" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D10)</f>
-        <v>2.777777778</v>
+        <v>2.739106754</v>
       </c>
       <c r="E10" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E10)</f>
-        <v>5.592592593</v>
+        <v>5.582244009</v>
       </c>
       <c r="F10" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F10)</f>
-        <v>5.740740741</v>
+        <v>5.747276688</v>
       </c>
       <c r="G10" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G10)</f>
-        <v>4.833333333</v>
+        <v>4.814814815</v>
       </c>
       <c r="H10" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H10)</f>
-        <v>3.305555556</v>
+        <v>3.352396514</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="7">
+        <f>AVERAGE('Ranking Per Race'!B$2:B11)</f>
+        <v>2.517647059</v>
+      </c>
+      <c r="C11" s="7">
+        <f>AVERAGE('Ranking Per Race'!C$2:C11)</f>
+        <v>3.403431373</v>
+      </c>
+      <c r="D11" s="7">
+        <f>AVERAGE('Ranking Per Race'!D$2:D11)</f>
+        <v>2.631862745</v>
+      </c>
+      <c r="E11" s="7">
+        <f>AVERAGE('Ranking Per Race'!E$2:E11)</f>
+        <v>5.557352941</v>
+      </c>
+      <c r="F11" s="7">
+        <f>AVERAGE('Ranking Per Race'!F$2:F11)</f>
+        <v>5.839215686</v>
+      </c>
+      <c r="G11" s="7">
+        <f>AVERAGE('Ranking Per Race'!G$2:G11)</f>
+        <v>4.8</v>
+      </c>
+      <c r="H11" s="7">
+        <f>AVERAGE('Ranking Per Race'!H$2:H11)</f>
+        <v>3.250490196</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="7">
+        <f>AVERAGE('Ranking Per Race'!B$2:B12)</f>
+        <v>2.470588235</v>
+      </c>
+      <c r="C12" s="7">
+        <f>AVERAGE('Ranking Per Race'!C$2:C12)</f>
+        <v>3.639483066</v>
+      </c>
+      <c r="D12" s="7">
+        <f>AVERAGE('Ranking Per Race'!D$2:D12)</f>
+        <v>2.483511586</v>
+      </c>
+      <c r="E12" s="7">
+        <f>AVERAGE('Ranking Per Race'!E$2:E12)</f>
+        <v>5.597593583</v>
+      </c>
+      <c r="F12" s="7">
+        <f>AVERAGE('Ranking Per Race'!F$2:F12)</f>
+        <v>5.808377897</v>
+      </c>
+      <c r="G12" s="7">
+        <f>AVERAGE('Ranking Per Race'!G$2:G12)</f>
+        <v>4.772727273</v>
+      </c>
+      <c r="H12" s="7">
+        <f>AVERAGE('Ranking Per Race'!H$2:H12)</f>
+        <v>3.22771836</v>
       </c>
     </row>
   </sheetData>
@@ -2055,7 +2338,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>14</v>
@@ -2064,7 +2347,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>17</v>
@@ -2250,31 +2533,31 @@
       </c>
       <c r="B7" s="7">
         <f>AVERAGE('Average Ranking'!B$2:B7)</f>
-        <v>1.740509259</v>
+        <v>1.731522331</v>
       </c>
       <c r="C7" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C7)</f>
-        <v>2.551388889</v>
+        <v>2.563916122</v>
       </c>
       <c r="D7" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D7)</f>
-        <v>3.13587963</v>
+        <v>3.126211874</v>
       </c>
       <c r="E7" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E7)</f>
-        <v>5.299537037</v>
+        <v>5.296949891</v>
       </c>
       <c r="F7" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F7)</f>
-        <v>5.168055556</v>
+        <v>5.169689542</v>
       </c>
       <c r="G7" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G7)</f>
-        <v>4.962268519</v>
+        <v>4.957638889</v>
       </c>
       <c r="H7" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H7)</f>
-        <v>5.142361111</v>
+        <v>5.154071351</v>
       </c>
     </row>
     <row r="8">
@@ -2283,31 +2566,31 @@
       </c>
       <c r="B8" s="7">
         <f>AVERAGE('Average Ranking'!B$2:B8)</f>
-        <v>1.835402494</v>
+        <v>1.821096772</v>
       </c>
       <c r="C8" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C8)</f>
-        <v>2.620578231</v>
+        <v>2.640519541</v>
       </c>
       <c r="D8" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D8)</f>
-        <v>3.130073696</v>
+        <v>3.114684207</v>
       </c>
       <c r="E8" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E8)</f>
-        <v>5.334977324</v>
+        <v>5.33085901</v>
       </c>
       <c r="F8" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F8)</f>
-        <v>5.225680272</v>
+        <v>5.228281313</v>
       </c>
       <c r="G8" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G8)</f>
-        <v>4.899631519</v>
+        <v>4.892261905</v>
       </c>
       <c r="H8" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H8)</f>
-        <v>4.953656463</v>
+        <v>4.972297252</v>
       </c>
     </row>
     <row r="9">
@@ -2316,31 +2599,31 @@
       </c>
       <c r="B9" s="7">
         <f>AVERAGE('Average Ranking'!B$2:B9)</f>
-        <v>1.915873016</v>
+        <v>1.898300362</v>
       </c>
       <c r="C9" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C9)</f>
-        <v>2.682328869</v>
+        <v>2.706824084</v>
       </c>
       <c r="D9" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D9)</f>
-        <v>3.113814484</v>
+        <v>3.094910568</v>
       </c>
       <c r="E9" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E9)</f>
-        <v>5.368625992</v>
+        <v>5.363567198</v>
       </c>
       <c r="F9" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F9)</f>
-        <v>5.270386905</v>
+        <v>5.273581933</v>
       </c>
       <c r="G9" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G9)</f>
-        <v>4.880927579</v>
+        <v>4.871875</v>
       </c>
       <c r="H9" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H9)</f>
-        <v>4.768043155</v>
+        <v>4.790940856</v>
       </c>
     </row>
     <row r="10">
@@ -2349,31 +2632,97 @@
       </c>
       <c r="B10" s="7">
         <f>AVERAGE('Average Ranking'!B$2:B10)</f>
-        <v>1.98489124</v>
+        <v>1.965276913</v>
       </c>
       <c r="C10" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C10)</f>
-        <v>2.741288213</v>
+        <v>2.768629396</v>
       </c>
       <c r="D10" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D10)</f>
-        <v>3.076477072</v>
+        <v>3.055376811</v>
       </c>
       <c r="E10" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E10)</f>
-        <v>5.39351117</v>
+        <v>5.387864621</v>
       </c>
       <c r="F10" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F10)</f>
-        <v>5.322648442</v>
+        <v>5.326214683</v>
       </c>
       <c r="G10" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G10)</f>
-        <v>4.87563933</v>
+        <v>4.865534979</v>
       </c>
       <c r="H10" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H10)</f>
-        <v>4.605544533</v>
+        <v>4.631102595</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="7">
+        <f>AVERAGE('Average Ranking'!B$2:B11)</f>
+        <v>2.020513928</v>
+      </c>
+      <c r="C11" s="7">
+        <f>AVERAGE('Average Ranking'!C$2:C11)</f>
+        <v>2.832109594</v>
+      </c>
+      <c r="D11" s="7">
+        <f>AVERAGE('Average Ranking'!D$2:D11)</f>
+        <v>3.013025405</v>
+      </c>
+      <c r="E11" s="7">
+        <f>AVERAGE('Average Ranking'!E$2:E11)</f>
+        <v>5.404813453</v>
+      </c>
+      <c r="F11" s="7">
+        <f>AVERAGE('Average Ranking'!F$2:F11)</f>
+        <v>5.377514784</v>
+      </c>
+      <c r="G11" s="7">
+        <f>AVERAGE('Average Ranking'!G$2:G11)</f>
+        <v>4.858981481</v>
+      </c>
+      <c r="H11" s="7">
+        <f>AVERAGE('Average Ranking'!H$2:H11)</f>
+        <v>4.493041355</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="7">
+        <f>AVERAGE('Average Ranking'!B$2:B12)</f>
+        <v>2.061429774</v>
+      </c>
+      <c r="C12" s="7">
+        <f>AVERAGE('Average Ranking'!C$2:C12)</f>
+        <v>2.905507182</v>
+      </c>
+      <c r="D12" s="7">
+        <f>AVERAGE('Average Ranking'!D$2:D12)</f>
+        <v>2.964887785</v>
+      </c>
+      <c r="E12" s="7">
+        <f>AVERAGE('Average Ranking'!E$2:E12)</f>
+        <v>5.422338919</v>
+      </c>
+      <c r="F12" s="7">
+        <f>AVERAGE('Average Ranking'!F$2:F12)</f>
+        <v>5.416684158</v>
+      </c>
+      <c r="G12" s="7">
+        <f>AVERAGE('Average Ranking'!G$2:G12)</f>
+        <v>4.85114019</v>
+      </c>
+      <c r="H12" s="7">
+        <f>AVERAGE('Average Ranking'!H$2:H12)</f>
+        <v>4.378011992</v>
       </c>
     </row>
   </sheetData>
@@ -2717,35 +3066,28 @@
     <row r="11">
       <c r="A11" s="6" t="str">
         <f>'Pre-Final Ranking'!A11</f>
-        <v/>
-      </c>
-      <c r="B11" s="6" t="str">
-        <f>'Pre-Final Ranking'!B11</f>
-        <v/>
-      </c>
-      <c r="C11" s="6" t="str">
-        <f>'Pre-Final Ranking'!C11</f>
-        <v/>
-      </c>
-      <c r="D11" s="6" t="str">
-        <f>'Pre-Final Ranking'!D11</f>
-        <v/>
-      </c>
-      <c r="E11" s="6" t="str">
-        <f>'Pre-Final Ranking'!E11</f>
-        <v/>
-      </c>
-      <c r="F11" s="6" t="str">
-        <f>'Pre-Final Ranking'!F11</f>
-        <v/>
-      </c>
-      <c r="G11" s="6" t="str">
-        <f>'Pre-Final Ranking'!G11</f>
-        <v/>
-      </c>
-      <c r="H11" s="6" t="str">
-        <f>'Pre-Final Ranking'!H11</f>
-        <v/>
+        <v>Brazil</v>
+      </c>
+      <c r="B11" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="C11" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="G11" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="H11" s="6">
+        <v>3.0</v>
       </c>
       <c r="I11" s="6" t="str">
         <f>'Pre-Final Ranking'!I11</f>
@@ -2755,35 +3097,28 @@
     <row r="12">
       <c r="A12" s="6" t="str">
         <f>'Pre-Final Ranking'!A12</f>
-        <v/>
-      </c>
-      <c r="B12" s="6" t="str">
-        <f>'Pre-Final Ranking'!B12</f>
-        <v/>
-      </c>
-      <c r="C12" s="6" t="str">
-        <f>'Pre-Final Ranking'!C12</f>
-        <v/>
-      </c>
-      <c r="D12" s="6" t="str">
-        <f>'Pre-Final Ranking'!D12</f>
-        <v/>
-      </c>
-      <c r="E12" s="6" t="str">
-        <f>'Pre-Final Ranking'!E12</f>
-        <v/>
-      </c>
-      <c r="F12" s="6" t="str">
-        <f>'Pre-Final Ranking'!F12</f>
-        <v/>
-      </c>
-      <c r="G12" s="6" t="str">
-        <f>'Pre-Final Ranking'!G12</f>
-        <v/>
-      </c>
-      <c r="H12" s="6" t="str">
-        <f>'Pre-Final Ranking'!H12</f>
-        <v/>
+        <v>Austria</v>
+      </c>
+      <c r="B12" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="H12" s="6">
+        <v>2.0</v>
       </c>
       <c r="I12" s="6" t="str">
         <f>'Pre-Final Ranking'!I12</f>

</xml_diff>

<commit_message>
jeddah and vegas power rankings
</commit_message>
<xml_diff>
--- a/The Alternative F1 Season 4 Power Rankings (Responses).xlsx
+++ b/The Alternative F1 Season 4 Power Rankings (Responses).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
   <si>
     <t>Timestamp</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Zandvoort</t>
+  </si>
+  <si>
+    <t>Jeddah</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
   </si>
   <si>
     <t>Race</t>
@@ -270,7 +276,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I37" displayName="Form_Responses" name="Form_Responses" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I40" displayName="Form_Responses" name="Form_Responses" id="1">
   <tableColumns count="9">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -1577,6 +1583,93 @@
         <v>3.0</v>
       </c>
     </row>
+    <row r="38" ht="22.5" customHeight="1">
+      <c r="A38" s="4">
+        <v>46030.73491990741</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="D38" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="E38" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="F38" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="G38" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="H38" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="I38" s="5">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="39" ht="22.5" customHeight="1">
+      <c r="A39" s="4">
+        <v>46030.73656068287</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D39" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="E39" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="F39" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="G39" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="H39" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="I39" s="5">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="40" ht="22.5" customHeight="1">
+      <c r="A40" s="4">
+        <v>46033.434448935186</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D40" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E40" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="F40" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="G40" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="H40" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="I40" s="5">
+        <v>4.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -1788,32 +1881,32 @@
         <v>26</v>
       </c>
       <c r="B7" s="7">
-        <f>AVERAGE('Form Responses 1'!C19:C40)</f>
-        <v>3.105263158</v>
+        <f>AVERAGE('Form Responses 1'!C19:C43)</f>
+        <v>3</v>
       </c>
       <c r="C7" s="7">
-        <f>AVERAGE('Form Responses 1'!D19:D40)</f>
-        <v>4.315789474</v>
+        <f>AVERAGE('Form Responses 1'!D19:D43)</f>
+        <v>4.318181818</v>
       </c>
       <c r="D7" s="7">
-        <f>AVERAGE('Form Responses 1'!E19:E40)</f>
-        <v>2.105263158</v>
+        <f>AVERAGE('Form Responses 1'!E19:E43)</f>
+        <v>2</v>
       </c>
       <c r="E7" s="7">
-        <f>AVERAGE('Form Responses 1'!F19:F40)</f>
-        <v>5.684210526</v>
+        <f>AVERAGE('Form Responses 1'!F19:F43)</f>
+        <v>5.454545455</v>
       </c>
       <c r="F7" s="7">
-        <f>AVERAGE('Form Responses 1'!G19:G40)</f>
-        <v>6.157894737</v>
+        <f>AVERAGE('Form Responses 1'!G19:G43)</f>
+        <v>6.181818182</v>
       </c>
       <c r="G7" s="7">
-        <f>AVERAGE('Form Responses 1'!H19:H40)</f>
-        <v>4.947368421</v>
+        <f>AVERAGE('Form Responses 1'!H19:H43)</f>
+        <v>5.181818182</v>
       </c>
       <c r="H7" s="7">
-        <f>AVERAGE('Form Responses 1'!I19:I40)</f>
-        <v>1.684210526</v>
+        <f>AVERAGE('Form Responses 1'!I19:I43)</f>
+        <v>1.863636364</v>
       </c>
     </row>
     <row r="8">
@@ -2012,6 +2105,72 @@
       <c r="H13" s="7">
         <f>AVERAGE('Form Responses 1'!I36:I37)</f>
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="7">
+        <f>AVERAGE('Form Responses 1'!C38:C40)</f>
+        <v>2.333333333</v>
+      </c>
+      <c r="C14" s="7">
+        <f>AVERAGE('Form Responses 1'!D38:D40)</f>
+        <v>4.333333333</v>
+      </c>
+      <c r="D14" s="7">
+        <f>AVERAGE('Form Responses 1'!E38:E40)</f>
+        <v>1.333333333</v>
+      </c>
+      <c r="E14" s="7">
+        <f>AVERAGE('Form Responses 1'!F38:F40)</f>
+        <v>4</v>
+      </c>
+      <c r="F14" s="7">
+        <f>AVERAGE('Form Responses 1'!G38:G40)</f>
+        <v>6.333333333</v>
+      </c>
+      <c r="G14" s="7">
+        <f>AVERAGE('Form Responses 1'!H38:H40)</f>
+        <v>6.666666667</v>
+      </c>
+      <c r="H14" s="7">
+        <f>AVERAGE('Form Responses 1'!I38:I40)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="7">
+        <f>AVERAGE('Form Responses 1'!C38:C40)</f>
+        <v>2.333333333</v>
+      </c>
+      <c r="C15" s="7">
+        <f>AVERAGE('Form Responses 1'!D38:D40)</f>
+        <v>4.333333333</v>
+      </c>
+      <c r="D15" s="7">
+        <f>AVERAGE('Form Responses 1'!E38:E40)</f>
+        <v>1.333333333</v>
+      </c>
+      <c r="E15" s="7">
+        <f>AVERAGE('Form Responses 1'!F38:F40)</f>
+        <v>4</v>
+      </c>
+      <c r="F15" s="7">
+        <f>AVERAGE('Form Responses 1'!G38:G40)</f>
+        <v>6.333333333</v>
+      </c>
+      <c r="G15" s="7">
+        <f>AVERAGE('Form Responses 1'!H38:H40)</f>
+        <v>6.666666667</v>
+      </c>
+      <c r="H15" s="7">
+        <f>AVERAGE('Form Responses 1'!I38:I40)</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2223,31 +2382,31 @@
       </c>
       <c r="B7" s="7">
         <f>AVERAGE('Ranking Per Race'!B$2:B7)</f>
-        <v>2.281432749</v>
+        <v>2.263888889</v>
       </c>
       <c r="C7" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C7)</f>
-        <v>3.024853801</v>
+        <v>3.025252525</v>
       </c>
       <c r="D7" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D7)</f>
-        <v>2.864766082</v>
+        <v>2.847222222</v>
       </c>
       <c r="E7" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E7)</f>
-        <v>5.558479532</v>
+        <v>5.52020202</v>
       </c>
       <c r="F7" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F7)</f>
-        <v>5.442982456</v>
+        <v>5.446969697</v>
       </c>
       <c r="G7" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G7)</f>
-        <v>4.449561404</v>
+        <v>4.488636364</v>
       </c>
       <c r="H7" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H7)</f>
-        <v>4.377923977</v>
+        <v>4.407828283</v>
       </c>
     </row>
     <row r="8">
@@ -2256,31 +2415,31 @@
       </c>
       <c r="B8" s="7">
         <f>AVERAGE('Ranking Per Race'!B$2:B8)</f>
-        <v>2.348370927</v>
+        <v>2.333333333</v>
       </c>
       <c r="C8" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C8)</f>
-        <v>3.128446115</v>
+        <v>3.128787879</v>
       </c>
       <c r="D8" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D8)</f>
-        <v>3.026942356</v>
+        <v>3.011904762</v>
       </c>
       <c r="E8" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E8)</f>
-        <v>5.514411028</v>
+        <v>5.481601732</v>
       </c>
       <c r="F8" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F8)</f>
-        <v>5.593984962</v>
+        <v>5.597402597</v>
       </c>
       <c r="G8" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G8)</f>
-        <v>4.492481203</v>
+        <v>4.525974026</v>
       </c>
       <c r="H8" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H8)</f>
-        <v>3.895363409</v>
+        <v>3.920995671</v>
       </c>
     </row>
     <row r="9">
@@ -2289,31 +2448,31 @@
       </c>
       <c r="B9" s="7">
         <f>AVERAGE('Ranking Per Race'!B$2:B9)</f>
-        <v>2.429824561</v>
+        <v>2.416666667</v>
       </c>
       <c r="C9" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C9)</f>
-        <v>3.195723684</v>
+        <v>3.196022727</v>
       </c>
       <c r="D9" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D9)</f>
-        <v>2.940241228</v>
+        <v>2.927083333</v>
       </c>
       <c r="E9" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E9)</f>
-        <v>5.575109649</v>
+        <v>5.546401515</v>
       </c>
       <c r="F9" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F9)</f>
-        <v>5.603070175</v>
+        <v>5.606060606</v>
       </c>
       <c r="G9" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G9)</f>
-        <v>4.722587719</v>
+        <v>4.751893939</v>
       </c>
       <c r="H9" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H9)</f>
-        <v>3.533442982</v>
+        <v>3.555871212</v>
       </c>
     </row>
     <row r="10">
@@ -2322,31 +2481,31 @@
       </c>
       <c r="B10" s="7">
         <f>AVERAGE('Ranking Per Race'!B$2:B10)</f>
-        <v>2.493177388</v>
+        <v>2.481481481</v>
       </c>
       <c r="C10" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C10)</f>
-        <v>3.285087719</v>
+        <v>3.285353535</v>
       </c>
       <c r="D10" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D10)</f>
-        <v>2.724658869</v>
+        <v>2.712962963</v>
       </c>
       <c r="E10" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E10)</f>
-        <v>5.566764133</v>
+        <v>5.541245791</v>
       </c>
       <c r="F10" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F10)</f>
-        <v>5.7582846</v>
+        <v>5.760942761</v>
       </c>
       <c r="G10" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G10)</f>
-        <v>4.808966862</v>
+        <v>4.835016835</v>
       </c>
       <c r="H10" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H10)</f>
-        <v>3.363060429</v>
+        <v>3.382996633</v>
       </c>
     </row>
     <row r="11">
@@ -2355,31 +2514,31 @@
       </c>
       <c r="B11" s="7">
         <f>AVERAGE('Ranking Per Race'!B$2:B11)</f>
-        <v>2.510526316</v>
+        <v>2.5</v>
       </c>
       <c r="C11" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C11)</f>
-        <v>3.423245614</v>
+        <v>3.423484848</v>
       </c>
       <c r="D11" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D11)</f>
-        <v>2.618859649</v>
+        <v>2.608333333</v>
       </c>
       <c r="E11" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E11)</f>
-        <v>5.543421053</v>
+        <v>5.520454545</v>
       </c>
       <c r="F11" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F11)</f>
-        <v>5.849122807</v>
+        <v>5.851515152</v>
       </c>
       <c r="G11" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G11)</f>
-        <v>4.794736842</v>
+        <v>4.818181818</v>
       </c>
       <c r="H11" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H11)</f>
-        <v>3.260087719</v>
+        <v>3.278030303</v>
       </c>
     </row>
     <row r="12">
@@ -2388,31 +2547,31 @@
       </c>
       <c r="B12" s="7">
         <f>AVERAGE('Ranking Per Race'!B$2:B12)</f>
-        <v>2.464114833</v>
+        <v>2.454545455</v>
       </c>
       <c r="C12" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C12)</f>
-        <v>3.657496013</v>
+        <v>3.657713499</v>
       </c>
       <c r="D12" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D12)</f>
-        <v>2.47169059</v>
+        <v>2.462121212</v>
       </c>
       <c r="E12" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E12)</f>
-        <v>5.58492823</v>
+        <v>5.564049587</v>
       </c>
       <c r="F12" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F12)</f>
-        <v>5.81738437</v>
+        <v>5.819559229</v>
       </c>
       <c r="G12" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G12)</f>
-        <v>4.767942584</v>
+        <v>4.789256198</v>
       </c>
       <c r="H12" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H12)</f>
-        <v>3.236443381</v>
+        <v>3.252754821</v>
       </c>
     </row>
     <row r="13">
@@ -2421,31 +2580,97 @@
       </c>
       <c r="B13" s="7">
         <f>AVERAGE('Ranking Per Race'!B$2:B13)</f>
-        <v>2.467105263</v>
+        <v>2.458333333</v>
       </c>
       <c r="C13" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C13)</f>
-        <v>3.852704678</v>
+        <v>3.85290404</v>
       </c>
       <c r="D13" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D13)</f>
-        <v>2.349049708</v>
+        <v>2.340277778</v>
       </c>
       <c r="E13" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E13)</f>
-        <v>5.494517544</v>
+        <v>5.475378788</v>
       </c>
       <c r="F13" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F13)</f>
-        <v>5.915935673</v>
+        <v>5.917929293</v>
       </c>
       <c r="G13" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G13)</f>
-        <v>4.745614035</v>
+        <v>4.765151515</v>
       </c>
       <c r="H13" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H13)</f>
-        <v>3.175073099</v>
+        <v>3.190025253</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="7">
+        <f>AVERAGE('Ranking Per Race'!B$2:B14)</f>
+        <v>2.448717949</v>
+      </c>
+      <c r="C14" s="7">
+        <f>AVERAGE('Ranking Per Race'!C$2:C14)</f>
+        <v>3.88986014</v>
+      </c>
+      <c r="D14" s="7">
+        <f>AVERAGE('Ranking Per Race'!D$2:D14)</f>
+        <v>2.262820513</v>
+      </c>
+      <c r="E14" s="7">
+        <f>AVERAGE('Ranking Per Race'!E$2:E14)</f>
+        <v>5.361888112</v>
+      </c>
+      <c r="F14" s="7">
+        <f>AVERAGE('Ranking Per Race'!F$2:F14)</f>
+        <v>5.94988345</v>
+      </c>
+      <c r="G14" s="7">
+        <f>AVERAGE('Ranking Per Race'!G$2:G14)</f>
+        <v>4.911421911</v>
+      </c>
+      <c r="H14" s="7">
+        <f>AVERAGE('Ranking Per Race'!H$2:H14)</f>
+        <v>3.175407925</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="7">
+        <f>AVERAGE('Ranking Per Race'!B$2:B15)</f>
+        <v>2.44047619</v>
+      </c>
+      <c r="C15" s="7">
+        <f>AVERAGE('Ranking Per Race'!C$2:C15)</f>
+        <v>3.921536797</v>
+      </c>
+      <c r="D15" s="7">
+        <f>AVERAGE('Ranking Per Race'!D$2:D15)</f>
+        <v>2.196428571</v>
+      </c>
+      <c r="E15" s="7">
+        <f>AVERAGE('Ranking Per Race'!E$2:E15)</f>
+        <v>5.26461039</v>
+      </c>
+      <c r="F15" s="7">
+        <f>AVERAGE('Ranking Per Race'!F$2:F15)</f>
+        <v>5.977272727</v>
+      </c>
+      <c r="G15" s="7">
+        <f>AVERAGE('Ranking Per Race'!G$2:G15)</f>
+        <v>5.036796537</v>
+      </c>
+      <c r="H15" s="7">
+        <f>AVERAGE('Ranking Per Race'!H$2:H15)</f>
+        <v>3.162878788</v>
       </c>
     </row>
   </sheetData>
@@ -2465,7 +2690,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>14</v>
@@ -2474,7 +2699,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>17</v>
@@ -2660,31 +2885,31 @@
       </c>
       <c r="B7" s="7">
         <f>AVERAGE('Average Ranking'!B$2:B7)</f>
-        <v>1.729544347</v>
+        <v>1.72662037</v>
       </c>
       <c r="C7" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C7)</f>
-        <v>2.569420078</v>
+        <v>2.569486532</v>
       </c>
       <c r="D7" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D7)</f>
-        <v>3.122599903</v>
+        <v>3.119675926</v>
       </c>
       <c r="E7" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E7)</f>
-        <v>5.293079922</v>
+        <v>5.286700337</v>
       </c>
       <c r="F7" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F7)</f>
-        <v>5.17244152</v>
+        <v>5.173106061</v>
       </c>
       <c r="G7" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G7)</f>
-        <v>4.956176901</v>
+        <v>4.962689394</v>
       </c>
       <c r="H7" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H7)</f>
-        <v>5.156737329</v>
+        <v>5.16172138</v>
       </c>
     </row>
     <row r="8">
@@ -2693,31 +2918,31 @@
       </c>
       <c r="B8" s="7">
         <f>AVERAGE('Average Ranking'!B$2:B8)</f>
-        <v>1.817948144</v>
+        <v>1.813293651</v>
       </c>
       <c r="C8" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C8)</f>
-        <v>2.64928094</v>
+        <v>2.649386724</v>
       </c>
       <c r="D8" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D8)</f>
-        <v>3.108934539</v>
+        <v>3.104280045</v>
       </c>
       <c r="E8" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E8)</f>
-        <v>5.324698651</v>
+        <v>5.314543393</v>
       </c>
       <c r="F8" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F8)</f>
-        <v>5.232662012</v>
+        <v>5.233719852</v>
       </c>
       <c r="G8" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G8)</f>
-        <v>4.889934658</v>
+        <v>4.900301484</v>
       </c>
       <c r="H8" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H8)</f>
-        <v>4.976541055</v>
+        <v>4.984474851</v>
       </c>
     </row>
     <row r="9">
@@ -2726,31 +2951,31 @@
       </c>
       <c r="B9" s="7">
         <f>AVERAGE('Average Ranking'!B$2:B9)</f>
-        <v>1.894432696</v>
+        <v>1.888715278</v>
       </c>
       <c r="C9" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C9)</f>
-        <v>2.717586283</v>
+        <v>2.717716225</v>
       </c>
       <c r="D9" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D9)</f>
-        <v>3.087847875</v>
+        <v>3.082130456</v>
       </c>
       <c r="E9" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E9)</f>
-        <v>5.356000026</v>
+        <v>5.343525658</v>
       </c>
       <c r="F9" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F9)</f>
-        <v>5.278963033</v>
+        <v>5.280262446</v>
       </c>
       <c r="G9" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G9)</f>
-        <v>4.869016291</v>
+        <v>4.881750541</v>
       </c>
       <c r="H9" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H9)</f>
-        <v>4.796153796</v>
+        <v>4.805899396</v>
       </c>
     </row>
     <row r="10">
@@ -2759,31 +2984,31 @@
       </c>
       <c r="B10" s="7">
         <f>AVERAGE('Average Ranking'!B$2:B10)</f>
-        <v>1.960959884</v>
+        <v>1.954578189</v>
       </c>
       <c r="C10" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C10)</f>
-        <v>2.780641999</v>
+        <v>2.780787037</v>
       </c>
       <c r="D10" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D10)</f>
-        <v>3.047493541</v>
+        <v>3.041111846</v>
       </c>
       <c r="E10" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E10)</f>
-        <v>5.37941826</v>
+        <v>5.365494562</v>
       </c>
       <c r="F10" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F10)</f>
-        <v>5.332220985</v>
+        <v>5.33367137</v>
       </c>
       <c r="G10" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G10)</f>
-        <v>4.862344132</v>
+        <v>4.876557907</v>
       </c>
       <c r="H10" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H10)</f>
-        <v>4.6369212</v>
+        <v>4.647799089</v>
       </c>
     </row>
     <row r="11">
@@ -2792,31 +3017,31 @@
       </c>
       <c r="B11" s="7">
         <f>AVERAGE('Average Ranking'!B$2:B11)</f>
-        <v>2.015916527</v>
+        <v>2.00912037</v>
       </c>
       <c r="C11" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C11)</f>
-        <v>2.84490236</v>
+        <v>2.845056818</v>
       </c>
       <c r="D11" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D11)</f>
-        <v>3.004630152</v>
+        <v>2.997833995</v>
       </c>
       <c r="E11" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E11)</f>
-        <v>5.395818539</v>
+        <v>5.38099056</v>
       </c>
       <c r="F11" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F11)</f>
-        <v>5.383911167</v>
+        <v>5.385455748</v>
       </c>
       <c r="G11" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G11)</f>
-        <v>4.855583403</v>
+        <v>4.870720298</v>
       </c>
       <c r="H11" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H11)</f>
-        <v>4.499237852</v>
+        <v>4.51082221</v>
       </c>
     </row>
     <row r="12">
@@ -2825,31 +3050,31 @@
       </c>
       <c r="B12" s="7">
         <f>AVERAGE('Average Ranking'!B$2:B12)</f>
-        <v>2.056661828</v>
+        <v>2.04961356</v>
       </c>
       <c r="C12" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C12)</f>
-        <v>2.91877451</v>
+        <v>2.918934698</v>
       </c>
       <c r="D12" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D12)</f>
-        <v>2.956181101</v>
+        <v>2.949132833</v>
       </c>
       <c r="E12" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E12)</f>
-        <v>5.413010329</v>
+        <v>5.39763229</v>
       </c>
       <c r="F12" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F12)</f>
-        <v>5.423317822</v>
+        <v>5.424919701</v>
       </c>
       <c r="G12" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G12)</f>
-        <v>4.847616056</v>
+        <v>4.863314471</v>
       </c>
       <c r="H12" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H12)</f>
-        <v>4.384438354</v>
+        <v>4.396452448</v>
       </c>
     </row>
     <row r="13">
@@ -2858,31 +3083,97 @@
       </c>
       <c r="B13" s="7">
         <f>AVERAGE('Average Ranking'!B$2:B13)</f>
-        <v>2.090865447</v>
+        <v>2.083673541</v>
       </c>
       <c r="C13" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C13)</f>
-        <v>2.996602024</v>
+        <v>2.996765477</v>
       </c>
       <c r="D13" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D13)</f>
-        <v>2.905586818</v>
+        <v>2.898394911</v>
       </c>
       <c r="E13" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E13)</f>
-        <v>5.419802597</v>
+        <v>5.404111165</v>
       </c>
       <c r="F13" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F13)</f>
-        <v>5.464369309</v>
+        <v>5.466003833</v>
       </c>
       <c r="G13" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G13)</f>
-        <v>4.839115887</v>
+        <v>4.855134225</v>
       </c>
       <c r="H13" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H13)</f>
-        <v>4.283657916</v>
+        <v>4.295916848</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="7">
+        <f>AVERAGE('Average Ranking'!B$2:B14)</f>
+        <v>2.11175388</v>
+      </c>
+      <c r="C14" s="7">
+        <f>AVERAGE('Average Ranking'!C$2:C14)</f>
+        <v>3.065465066</v>
+      </c>
+      <c r="D14" s="7">
+        <f>AVERAGE('Average Ranking'!D$2:D14)</f>
+        <v>2.849504573</v>
+      </c>
+      <c r="E14" s="7">
+        <f>AVERAGE('Average Ranking'!E$2:E14)</f>
+        <v>5.400863238</v>
+      </c>
+      <c r="F14" s="7">
+        <f>AVERAGE('Average Ranking'!F$2:F14)</f>
+        <v>5.503225342</v>
+      </c>
+      <c r="G14" s="7">
+        <f>AVERAGE('Average Ranking'!G$2:G14)</f>
+        <v>4.859464047</v>
+      </c>
+      <c r="H14" s="7">
+        <f>AVERAGE('Average Ranking'!H$2:H14)</f>
+        <v>4.209723854</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="7">
+        <f>AVERAGE('Average Ranking'!B$2:B15)</f>
+        <v>2.135234045</v>
+      </c>
+      <c r="C15" s="7">
+        <f>AVERAGE('Average Ranking'!C$2:C15)</f>
+        <v>3.126613047</v>
+      </c>
+      <c r="D15" s="7">
+        <f>AVERAGE('Average Ranking'!D$2:D15)</f>
+        <v>2.802856287</v>
+      </c>
+      <c r="E15" s="7">
+        <f>AVERAGE('Average Ranking'!E$2:E15)</f>
+        <v>5.391130891</v>
+      </c>
+      <c r="F15" s="7">
+        <f>AVERAGE('Average Ranking'!F$2:F15)</f>
+        <v>5.53708587</v>
+      </c>
+      <c r="G15" s="7">
+        <f>AVERAGE('Average Ranking'!G$2:G15)</f>
+        <v>4.872130653</v>
+      </c>
+      <c r="H15" s="7">
+        <f>AVERAGE('Average Ranking'!H$2:H15)</f>
+        <v>4.134949206</v>
       </c>
     </row>
   </sheetData>
@@ -3319,35 +3610,28 @@
     <row r="14">
       <c r="A14" s="6" t="str">
         <f>'Pre-Final Ranking'!A14</f>
-        <v/>
-      </c>
-      <c r="B14" s="6" t="str">
-        <f>'Pre-Final Ranking'!B14</f>
-        <v/>
-      </c>
-      <c r="C14" s="6" t="str">
-        <f>'Pre-Final Ranking'!C14</f>
-        <v/>
-      </c>
-      <c r="D14" s="6" t="str">
-        <f>'Pre-Final Ranking'!D14</f>
-        <v/>
-      </c>
-      <c r="E14" s="6" t="str">
-        <f>'Pre-Final Ranking'!E14</f>
-        <v/>
-      </c>
-      <c r="F14" s="6" t="str">
-        <f>'Pre-Final Ranking'!F14</f>
-        <v/>
-      </c>
-      <c r="G14" s="6" t="str">
-        <f>'Pre-Final Ranking'!G14</f>
-        <v/>
-      </c>
-      <c r="H14" s="6" t="str">
-        <f>'Pre-Final Ranking'!H14</f>
-        <v/>
+        <v>Jeddah</v>
+      </c>
+      <c r="B14" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="C14" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>2.0</v>
       </c>
       <c r="I14" s="6" t="str">
         <f>'Pre-Final Ranking'!I14</f>
@@ -3357,35 +3641,28 @@
     <row r="15">
       <c r="A15" s="6" t="str">
         <f>'Pre-Final Ranking'!A15</f>
-        <v/>
-      </c>
-      <c r="B15" s="6" t="str">
-        <f>'Pre-Final Ranking'!B15</f>
-        <v/>
-      </c>
-      <c r="C15" s="6" t="str">
-        <f>'Pre-Final Ranking'!C15</f>
-        <v/>
-      </c>
-      <c r="D15" s="6" t="str">
-        <f>'Pre-Final Ranking'!D15</f>
-        <v/>
-      </c>
-      <c r="E15" s="6" t="str">
-        <f>'Pre-Final Ranking'!E15</f>
-        <v/>
-      </c>
-      <c r="F15" s="6" t="str">
-        <f>'Pre-Final Ranking'!F15</f>
-        <v/>
-      </c>
-      <c r="G15" s="6" t="str">
-        <f>'Pre-Final Ranking'!G15</f>
-        <v/>
-      </c>
-      <c r="H15" s="6" t="str">
-        <f>'Pre-Final Ranking'!H15</f>
-        <v/>
+        <v>Las Vegas</v>
+      </c>
+      <c r="B15" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="C15" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="G15" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1.0</v>
       </c>
       <c r="I15" s="6" t="str">
         <f>'Pre-Final Ranking'!I15</f>

</xml_diff>

<commit_message>
abu dhabi power Rankings
</commit_message>
<xml_diff>
--- a/The Alternative F1 Season 4 Power Rankings (Responses).xlsx
+++ b/The Alternative F1 Season 4 Power Rankings (Responses).xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Ranking Per Race" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Average Ranking" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Pre-Final Ranking" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Final Ranking" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="Ranking Per Race" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="Average Ranking" sheetId="3" r:id="rId7"/>
+    <sheet state="visible" name="Pre-Final Ranking" sheetId="4" r:id="rId8"/>
+    <sheet state="visible" name="Final Ranking" sheetId="5" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="38">
   <si>
     <t>Timestamp</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>Abu Dhabi</t>
   </si>
   <si>
     <t>Race</t>
@@ -275,8 +278,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I40" displayName="Form_Responses" name="Form_Responses" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I42" displayName="Form_Responses" name="Form_Responses" id="1">
   <tableColumns count="9">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -1670,6 +1677,64 @@
         <v>4.0</v>
       </c>
     </row>
+    <row r="41" ht="22.5" customHeight="1">
+      <c r="A41" s="4">
+        <v>46038.79511320602</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D41" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E41" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="F41" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="G41" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="H41" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="I41" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="42" ht="22.5" customHeight="1">
+      <c r="A42" s="4">
+        <v>46038.79693108796</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D42" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E42" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="F42" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="G42" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="H42" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="I42" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -1881,32 +1946,32 @@
         <v>26</v>
       </c>
       <c r="B7" s="7">
-        <f>AVERAGE('Form Responses 1'!C19:C43)</f>
+        <f>AVERAGE('Form Responses 1'!C19:C45)</f>
         <v>3</v>
       </c>
       <c r="C7" s="7">
-        <f>AVERAGE('Form Responses 1'!D19:D43)</f>
-        <v>4.318181818</v>
+        <f>AVERAGE('Form Responses 1'!D19:D45)</f>
+        <v>4.5</v>
       </c>
       <c r="D7" s="7">
-        <f>AVERAGE('Form Responses 1'!E19:E43)</f>
+        <f>AVERAGE('Form Responses 1'!E19:E45)</f>
         <v>2</v>
       </c>
       <c r="E7" s="7">
-        <f>AVERAGE('Form Responses 1'!F19:F43)</f>
-        <v>5.454545455</v>
+        <f>AVERAGE('Form Responses 1'!F19:F45)</f>
+        <v>5.333333333</v>
       </c>
       <c r="F7" s="7">
-        <f>AVERAGE('Form Responses 1'!G19:G43)</f>
-        <v>6.181818182</v>
+        <f>AVERAGE('Form Responses 1'!G19:G45)</f>
+        <v>6.208333333</v>
       </c>
       <c r="G7" s="7">
-        <f>AVERAGE('Form Responses 1'!H19:H43)</f>
-        <v>5.181818182</v>
+        <f>AVERAGE('Form Responses 1'!H19:H45)</f>
+        <v>5.166666667</v>
       </c>
       <c r="H7" s="7">
-        <f>AVERAGE('Form Responses 1'!I19:I43)</f>
-        <v>1.863636364</v>
+        <f>AVERAGE('Form Responses 1'!I19:I45)</f>
+        <v>1.791666667</v>
       </c>
     </row>
     <row r="8">
@@ -2171,6 +2236,39 @@
       <c r="H15" s="7">
         <f>AVERAGE('Form Responses 1'!I38:I40)</f>
         <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="7">
+        <f>AVERAGE('Form Responses 1'!C41:C42)</f>
+        <v>3</v>
+      </c>
+      <c r="C16" s="7">
+        <f>AVERAGE('Form Responses 1'!D41:D42)</f>
+        <v>6.5</v>
+      </c>
+      <c r="D16" s="7">
+        <f>AVERAGE('Form Responses 1'!E41:E42)</f>
+        <v>2</v>
+      </c>
+      <c r="E16" s="7">
+        <f>AVERAGE('Form Responses 1'!F41:F42)</f>
+        <v>4</v>
+      </c>
+      <c r="F16" s="7">
+        <f>AVERAGE('Form Responses 1'!G41:G42)</f>
+        <v>6.5</v>
+      </c>
+      <c r="G16" s="7">
+        <f>AVERAGE('Form Responses 1'!H41:H42)</f>
+        <v>5</v>
+      </c>
+      <c r="H16" s="7">
+        <f>AVERAGE('Form Responses 1'!I41:I42)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2386,7 +2484,7 @@
       </c>
       <c r="C7" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C7)</f>
-        <v>3.025252525</v>
+        <v>3.055555556</v>
       </c>
       <c r="D7" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D7)</f>
@@ -2394,19 +2492,19 @@
       </c>
       <c r="E7" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E7)</f>
-        <v>5.52020202</v>
+        <v>5.5</v>
       </c>
       <c r="F7" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F7)</f>
-        <v>5.446969697</v>
+        <v>5.451388889</v>
       </c>
       <c r="G7" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G7)</f>
-        <v>4.488636364</v>
+        <v>4.486111111</v>
       </c>
       <c r="H7" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H7)</f>
-        <v>4.407828283</v>
+        <v>4.395833333</v>
       </c>
     </row>
     <row r="8">
@@ -2419,7 +2517,7 @@
       </c>
       <c r="C8" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C8)</f>
-        <v>3.128787879</v>
+        <v>3.154761905</v>
       </c>
       <c r="D8" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D8)</f>
@@ -2427,19 +2525,19 @@
       </c>
       <c r="E8" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E8)</f>
-        <v>5.481601732</v>
+        <v>5.464285714</v>
       </c>
       <c r="F8" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F8)</f>
-        <v>5.597402597</v>
+        <v>5.601190476</v>
       </c>
       <c r="G8" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G8)</f>
-        <v>4.525974026</v>
+        <v>4.523809524</v>
       </c>
       <c r="H8" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H8)</f>
-        <v>3.920995671</v>
+        <v>3.910714286</v>
       </c>
     </row>
     <row r="9">
@@ -2452,7 +2550,7 @@
       </c>
       <c r="C9" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C9)</f>
-        <v>3.196022727</v>
+        <v>3.21875</v>
       </c>
       <c r="D9" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D9)</f>
@@ -2460,19 +2558,19 @@
       </c>
       <c r="E9" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E9)</f>
-        <v>5.546401515</v>
+        <v>5.53125</v>
       </c>
       <c r="F9" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F9)</f>
-        <v>5.606060606</v>
+        <v>5.609375</v>
       </c>
       <c r="G9" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G9)</f>
-        <v>4.751893939</v>
+        <v>4.75</v>
       </c>
       <c r="H9" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H9)</f>
-        <v>3.555871212</v>
+        <v>3.546875</v>
       </c>
     </row>
     <row r="10">
@@ -2485,7 +2583,7 @@
       </c>
       <c r="C10" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C10)</f>
-        <v>3.285353535</v>
+        <v>3.305555556</v>
       </c>
       <c r="D10" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D10)</f>
@@ -2493,19 +2591,19 @@
       </c>
       <c r="E10" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E10)</f>
-        <v>5.541245791</v>
+        <v>5.527777778</v>
       </c>
       <c r="F10" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F10)</f>
-        <v>5.760942761</v>
+        <v>5.763888889</v>
       </c>
       <c r="G10" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G10)</f>
-        <v>4.835016835</v>
+        <v>4.833333333</v>
       </c>
       <c r="H10" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H10)</f>
-        <v>3.382996633</v>
+        <v>3.375</v>
       </c>
     </row>
     <row r="11">
@@ -2518,7 +2616,7 @@
       </c>
       <c r="C11" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C11)</f>
-        <v>3.423484848</v>
+        <v>3.441666667</v>
       </c>
       <c r="D11" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D11)</f>
@@ -2526,19 +2624,19 @@
       </c>
       <c r="E11" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E11)</f>
-        <v>5.520454545</v>
+        <v>5.508333333</v>
       </c>
       <c r="F11" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F11)</f>
-        <v>5.851515152</v>
+        <v>5.854166667</v>
       </c>
       <c r="G11" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G11)</f>
-        <v>4.818181818</v>
+        <v>4.816666667</v>
       </c>
       <c r="H11" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H11)</f>
-        <v>3.278030303</v>
+        <v>3.270833333</v>
       </c>
     </row>
     <row r="12">
@@ -2551,7 +2649,7 @@
       </c>
       <c r="C12" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C12)</f>
-        <v>3.657713499</v>
+        <v>3.674242424</v>
       </c>
       <c r="D12" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D12)</f>
@@ -2559,19 +2657,19 @@
       </c>
       <c r="E12" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E12)</f>
-        <v>5.564049587</v>
+        <v>5.553030303</v>
       </c>
       <c r="F12" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F12)</f>
-        <v>5.819559229</v>
+        <v>5.821969697</v>
       </c>
       <c r="G12" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G12)</f>
-        <v>4.789256198</v>
+        <v>4.787878788</v>
       </c>
       <c r="H12" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H12)</f>
-        <v>3.252754821</v>
+        <v>3.246212121</v>
       </c>
     </row>
     <row r="13">
@@ -2584,7 +2682,7 @@
       </c>
       <c r="C13" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C13)</f>
-        <v>3.85290404</v>
+        <v>3.868055556</v>
       </c>
       <c r="D13" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D13)</f>
@@ -2592,19 +2690,19 @@
       </c>
       <c r="E13" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E13)</f>
-        <v>5.475378788</v>
+        <v>5.465277778</v>
       </c>
       <c r="F13" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F13)</f>
-        <v>5.917929293</v>
+        <v>5.920138889</v>
       </c>
       <c r="G13" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G13)</f>
-        <v>4.765151515</v>
+        <v>4.763888889</v>
       </c>
       <c r="H13" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H13)</f>
-        <v>3.190025253</v>
+        <v>3.184027778</v>
       </c>
     </row>
     <row r="14">
@@ -2617,7 +2715,7 @@
       </c>
       <c r="C14" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C14)</f>
-        <v>3.88986014</v>
+        <v>3.903846154</v>
       </c>
       <c r="D14" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D14)</f>
@@ -2625,19 +2723,19 @@
       </c>
       <c r="E14" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E14)</f>
-        <v>5.361888112</v>
+        <v>5.352564103</v>
       </c>
       <c r="F14" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F14)</f>
-        <v>5.94988345</v>
+        <v>5.951923077</v>
       </c>
       <c r="G14" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G14)</f>
-        <v>4.911421911</v>
+        <v>4.91025641</v>
       </c>
       <c r="H14" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H14)</f>
-        <v>3.175407925</v>
+        <v>3.169871795</v>
       </c>
     </row>
     <row r="15">
@@ -2650,7 +2748,7 @@
       </c>
       <c r="C15" s="7">
         <f>AVERAGE('Ranking Per Race'!C$2:C15)</f>
-        <v>3.921536797</v>
+        <v>3.93452381</v>
       </c>
       <c r="D15" s="7">
         <f>AVERAGE('Ranking Per Race'!D$2:D15)</f>
@@ -2658,19 +2756,52 @@
       </c>
       <c r="E15" s="7">
         <f>AVERAGE('Ranking Per Race'!E$2:E15)</f>
-        <v>5.26461039</v>
+        <v>5.255952381</v>
       </c>
       <c r="F15" s="7">
         <f>AVERAGE('Ranking Per Race'!F$2:F15)</f>
-        <v>5.977272727</v>
+        <v>5.979166667</v>
       </c>
       <c r="G15" s="7">
         <f>AVERAGE('Ranking Per Race'!G$2:G15)</f>
-        <v>5.036796537</v>
+        <v>5.035714286</v>
       </c>
       <c r="H15" s="7">
         <f>AVERAGE('Ranking Per Race'!H$2:H15)</f>
-        <v>3.162878788</v>
+        <v>3.157738095</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="7">
+        <f>AVERAGE('Ranking Per Race'!B$2:B16)</f>
+        <v>2.477777778</v>
+      </c>
+      <c r="C16" s="7">
+        <f>AVERAGE('Ranking Per Race'!C$2:C16)</f>
+        <v>4.105555556</v>
+      </c>
+      <c r="D16" s="7">
+        <f>AVERAGE('Ranking Per Race'!D$2:D16)</f>
+        <v>2.183333333</v>
+      </c>
+      <c r="E16" s="7">
+        <f>AVERAGE('Ranking Per Race'!E$2:E16)</f>
+        <v>5.172222222</v>
+      </c>
+      <c r="F16" s="7">
+        <f>AVERAGE('Ranking Per Race'!F$2:F16)</f>
+        <v>6.013888889</v>
+      </c>
+      <c r="G16" s="7">
+        <f>AVERAGE('Ranking Per Race'!G$2:G16)</f>
+        <v>5.033333333</v>
+      </c>
+      <c r="H16" s="7">
+        <f>AVERAGE('Ranking Per Race'!H$2:H16)</f>
+        <v>3.013888889</v>
       </c>
     </row>
   </sheetData>
@@ -2690,7 +2821,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>14</v>
@@ -2699,7 +2830,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>17</v>
@@ -2889,7 +3020,7 @@
       </c>
       <c r="C7" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C7)</f>
-        <v>2.569486532</v>
+        <v>2.574537037</v>
       </c>
       <c r="D7" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D7)</f>
@@ -2897,19 +3028,19 @@
       </c>
       <c r="E7" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E7)</f>
-        <v>5.286700337</v>
+        <v>5.283333333</v>
       </c>
       <c r="F7" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F7)</f>
-        <v>5.173106061</v>
+        <v>5.173842593</v>
       </c>
       <c r="G7" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G7)</f>
-        <v>4.962689394</v>
+        <v>4.962268519</v>
       </c>
       <c r="H7" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H7)</f>
-        <v>5.16172138</v>
+        <v>5.159722222</v>
       </c>
     </row>
     <row r="8">
@@ -2922,7 +3053,7 @@
       </c>
       <c r="C8" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C8)</f>
-        <v>2.649386724</v>
+        <v>2.657426304</v>
       </c>
       <c r="D8" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D8)</f>
@@ -2930,19 +3061,19 @@
       </c>
       <c r="E8" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E8)</f>
-        <v>5.314543393</v>
+        <v>5.309183673</v>
       </c>
       <c r="F8" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F8)</f>
-        <v>5.233719852</v>
+        <v>5.23489229</v>
       </c>
       <c r="G8" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G8)</f>
-        <v>4.900301484</v>
+        <v>4.899631519</v>
       </c>
       <c r="H8" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H8)</f>
-        <v>4.984474851</v>
+        <v>4.981292517</v>
       </c>
     </row>
     <row r="9">
@@ -2955,7 +3086,7 @@
       </c>
       <c r="C9" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C9)</f>
-        <v>2.717716225</v>
+        <v>2.727591766</v>
       </c>
       <c r="D9" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D9)</f>
@@ -2963,19 +3094,19 @@
       </c>
       <c r="E9" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E9)</f>
-        <v>5.343525658</v>
+        <v>5.336941964</v>
       </c>
       <c r="F9" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F9)</f>
-        <v>5.280262446</v>
+        <v>5.281702629</v>
       </c>
       <c r="G9" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G9)</f>
-        <v>4.881750541</v>
+        <v>4.880927579</v>
       </c>
       <c r="H9" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H9)</f>
-        <v>4.805899396</v>
+        <v>4.801990327</v>
       </c>
     </row>
     <row r="10">
@@ -2988,7 +3119,7 @@
       </c>
       <c r="C10" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C10)</f>
-        <v>2.780787037</v>
+        <v>2.791809965</v>
       </c>
       <c r="D10" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D10)</f>
@@ -2996,19 +3127,19 @@
       </c>
       <c r="E10" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E10)</f>
-        <v>5.365494562</v>
+        <v>5.358145944</v>
       </c>
       <c r="F10" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F10)</f>
-        <v>5.33367137</v>
+        <v>5.33527888</v>
       </c>
       <c r="G10" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G10)</f>
-        <v>4.876557907</v>
+        <v>4.87563933</v>
       </c>
       <c r="H10" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H10)</f>
-        <v>4.647799089</v>
+        <v>4.643435847</v>
       </c>
     </row>
     <row r="11">
@@ -3021,7 +3152,7 @@
       </c>
       <c r="C11" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C11)</f>
-        <v>2.845056818</v>
+        <v>2.856795635</v>
       </c>
       <c r="D11" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D11)</f>
@@ -3029,19 +3160,19 @@
       </c>
       <c r="E11" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E11)</f>
-        <v>5.38099056</v>
+        <v>5.373164683</v>
       </c>
       <c r="F11" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F11)</f>
-        <v>5.385455748</v>
+        <v>5.387167659</v>
       </c>
       <c r="G11" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G11)</f>
-        <v>4.870720298</v>
+        <v>4.869742063</v>
       </c>
       <c r="H11" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H11)</f>
-        <v>4.51082221</v>
+        <v>4.506175595</v>
       </c>
     </row>
     <row r="12">
@@ -3054,7 +3185,7 @@
       </c>
       <c r="C12" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C12)</f>
-        <v>2.918934698</v>
+        <v>2.931108979</v>
       </c>
       <c r="D12" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D12)</f>
@@ -3062,19 +3193,19 @@
       </c>
       <c r="E12" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E12)</f>
-        <v>5.39763229</v>
+        <v>5.389516103</v>
       </c>
       <c r="F12" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F12)</f>
-        <v>5.424919701</v>
+        <v>5.426695117</v>
       </c>
       <c r="G12" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G12)</f>
-        <v>4.863314471</v>
+        <v>4.862299948</v>
       </c>
       <c r="H12" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H12)</f>
-        <v>4.396452448</v>
+        <v>4.391633461</v>
       </c>
     </row>
     <row r="13">
@@ -3087,7 +3218,7 @@
       </c>
       <c r="C13" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C13)</f>
-        <v>2.996765477</v>
+        <v>3.009187861</v>
       </c>
       <c r="D13" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D13)</f>
@@ -3095,19 +3226,19 @@
       </c>
       <c r="E13" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E13)</f>
-        <v>5.404111165</v>
+        <v>5.395829576</v>
       </c>
       <c r="F13" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F13)</f>
-        <v>5.466003833</v>
+        <v>5.467815431</v>
       </c>
       <c r="G13" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G13)</f>
-        <v>4.855134225</v>
+        <v>4.854099026</v>
       </c>
       <c r="H13" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H13)</f>
-        <v>4.295916848</v>
+        <v>4.290999654</v>
       </c>
     </row>
     <row r="14">
@@ -3120,7 +3251,7 @@
       </c>
       <c r="C14" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C14)</f>
-        <v>3.065465066</v>
+        <v>3.078007729</v>
       </c>
       <c r="D14" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D14)</f>
@@ -3128,19 +3259,19 @@
       </c>
       <c r="E14" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E14)</f>
-        <v>5.400863238</v>
+        <v>5.392501462</v>
       </c>
       <c r="F14" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F14)</f>
-        <v>5.503225342</v>
+        <v>5.505054481</v>
       </c>
       <c r="G14" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G14)</f>
-        <v>4.859464047</v>
+        <v>4.858418825</v>
       </c>
       <c r="H14" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H14)</f>
-        <v>4.209723854</v>
+        <v>4.20475905</v>
       </c>
     </row>
     <row r="15">
@@ -3153,7 +3284,7 @@
       </c>
       <c r="C15" s="7">
         <f>AVERAGE('Average Ranking'!C$2:C15)</f>
-        <v>3.126613047</v>
+        <v>3.139187449</v>
       </c>
       <c r="D15" s="7">
         <f>AVERAGE('Average Ranking'!D$2:D15)</f>
@@ -3161,19 +3292,52 @@
       </c>
       <c r="E15" s="7">
         <f>AVERAGE('Average Ranking'!E$2:E15)</f>
-        <v>5.391130891</v>
+        <v>5.382747956</v>
       </c>
       <c r="F15" s="7">
         <f>AVERAGE('Average Ranking'!F$2:F15)</f>
-        <v>5.53708587</v>
+        <v>5.538919637</v>
       </c>
       <c r="G15" s="7">
         <f>AVERAGE('Average Ranking'!G$2:G15)</f>
-        <v>4.872130653</v>
+        <v>4.871082786</v>
       </c>
       <c r="H15" s="7">
         <f>AVERAGE('Average Ranking'!H$2:H15)</f>
-        <v>4.134949206</v>
+        <v>4.129971839</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="7">
+        <f>AVERAGE('Average Ranking'!B$2:B16)</f>
+        <v>2.158070294</v>
+      </c>
+      <c r="C16" s="7">
+        <f>AVERAGE('Average Ranking'!C$2:C16)</f>
+        <v>3.20361199</v>
+      </c>
+      <c r="D16" s="7">
+        <f>AVERAGE('Average Ranking'!D$2:D16)</f>
+        <v>2.761554757</v>
+      </c>
+      <c r="E16" s="7">
+        <f>AVERAGE('Average Ranking'!E$2:E16)</f>
+        <v>5.368712907</v>
+      </c>
+      <c r="F16" s="7">
+        <f>AVERAGE('Average Ranking'!F$2:F16)</f>
+        <v>5.570584254</v>
+      </c>
+      <c r="G16" s="7">
+        <f>AVERAGE('Average Ranking'!G$2:G16)</f>
+        <v>4.881899489</v>
+      </c>
+      <c r="H16" s="7">
+        <f>AVERAGE('Average Ranking'!H$2:H16)</f>
+        <v>4.055566309</v>
       </c>
     </row>
   </sheetData>
@@ -3672,35 +3836,28 @@
     <row r="16">
       <c r="A16" s="6" t="str">
         <f>'Pre-Final Ranking'!A16</f>
-        <v/>
-      </c>
-      <c r="B16" s="6" t="str">
-        <f>'Pre-Final Ranking'!B16</f>
-        <v/>
-      </c>
-      <c r="C16" s="6" t="str">
-        <f>'Pre-Final Ranking'!C16</f>
-        <v/>
-      </c>
-      <c r="D16" s="6" t="str">
-        <f>'Pre-Final Ranking'!D16</f>
-        <v/>
-      </c>
-      <c r="E16" s="6" t="str">
-        <f>'Pre-Final Ranking'!E16</f>
-        <v/>
-      </c>
-      <c r="F16" s="6" t="str">
-        <f>'Pre-Final Ranking'!F16</f>
-        <v/>
-      </c>
-      <c r="G16" s="6" t="str">
-        <f>'Pre-Final Ranking'!G16</f>
-        <v/>
-      </c>
-      <c r="H16" s="6" t="str">
-        <f>'Pre-Final Ranking'!H16</f>
-        <v/>
+        <v>Abu Dhabi</v>
+      </c>
+      <c r="B16" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="C16" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="D16" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="E16" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="F16" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="G16" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1.0</v>
       </c>
       <c r="I16" s="6" t="str">
         <f>'Pre-Final Ranking'!I16</f>

</xml_diff>